<commit_message>
Ajuste Registro de Cotización Elementos Relacionados Bien/Servicio
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Selección para carga de tipo Bien</t>
   </si>
@@ -86,31 +86,7 @@
     <t>Campo para descripcion del Servicio</t>
   </si>
   <si>
-    <t>Campo selección para unidad  del Servicio</t>
-  </si>
-  <si>
-    <t>Cantidad en años para T.E.</t>
-  </si>
-  <si>
-    <t>Cantidad en meses para T.E.</t>
-  </si>
-  <si>
-    <t>Cantidad en días  para T.E.</t>
-  </si>
-  <si>
     <t>Campo para cantidad  del Servicio</t>
-  </si>
-  <si>
-    <t>Tiempo Ejecucion</t>
-  </si>
-  <si>
-    <t>Años</t>
-  </si>
-  <si>
-    <t>Meses</t>
-  </si>
-  <si>
-    <t>Dias</t>
   </si>
   <si>
     <t>2 - SERVICIO</t>
@@ -244,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,18 +246,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -365,21 +329,21 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,25 +444,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,30 +478,12 @@
       <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -550,73 +496,30 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>456465.45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:G2"/>
-  </mergeCells>
-  <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="whole">
-      <formula1>0</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4" type="list">
-      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12"</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4" type="list">
-      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30"</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4" type="list">
       <formula1>"2 - SERVICIO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4" type="decimal">
       <formula1>0</formula1>
       <formula2>1.11111111111111E+015</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Ajuste presentación de adendas de modificación info/cambio y plugin
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -65,7 +65,7 @@
     <t>DESCRIPCION BIEN 1</t>
   </si>
   <si>
-    <t>3 - CENTIMETRO</t>
+    <t>35 - DECAGRAMO</t>
   </si>
   <si>
     <t>BIEN 2</t>
@@ -74,7 +74,7 @@
     <t>DESCRIPCION BIEN 2</t>
   </si>
   <si>
-    <t>5 - GRAMO</t>
+    <t>4 - KILOGRAMO</t>
   </si>
   <si>
     <t>Selección para carga de tipo Servicio</t>
@@ -334,16 +334,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,8 +415,8 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
       <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -427,6 +427,10 @@
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E4" type="decimal">
       <formula1>0</formula1>
       <formula2>1.11111111111111E+015</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3" type="list">
+      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD,14 - CENTILITRO,15 - MILILITRO,16 - KILÓMETRO CUADRADO,17 - HECTÓMETRO CUADRADO,18 - DECÁMETRO CUADRADO,19 - METRO CUADRADO,20 - DECÍMETRO CUADRADO,21 - CENTÍMETRO CUADRADO,22 - MILÍMETRO CUADRADO,23 - KILÓMETRO CÚBICO,24 - HECTÓMETRO CÚBICO,25 - DECÁMETRO CÚBICO,26 - METRO CÚBICO,27 - DECÍMETRO CÚBICO,28 - CENTÍMETRO CÚBICO,29 - MILÍMETRO CÚBICO,30 - HECTÓMETRO,31 - DECÁMETRO,32 - DECÍMETRO,33 - MILÍMETRO,34 - HECTOGRAMO,35 - DECAGRAMO,36 - DECIGRAMO,37 - CENTIGRAMO,38 - MILIGRAMO,39 - KILOLITRO,40 - HECTOLITRO,41 - DECALITRO,42 - DECILITRO,"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -452,17 +456,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Carga Ultima Versión del Sistemá ÁGORA
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/relacionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -334,16 +334,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,11 +415,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="3">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A4" type="list">
       <formula1>"1 - BIEN"</formula1>
       <formula2>0</formula2>
@@ -428,8 +424,8 @@
       <formula1>0</formula1>
       <formula2>1.11111111111111E+015</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD,14 - CENTILITRO,15 - MILILITRO,16 - KILÓMETRO CUADRADO,17 - HECTÓMETRO CUADRADO,18 - DECÁMETRO CUADRADO,19 - METRO CUADRADO,20 - DECÍMETRO CUADRADO,21 - CENTÍMETRO CUADRADO,22 - MILÍMETRO CUADRADO,23 - KILÓMETRO CÚBICO,24 - HECTÓMETRO CÚBICO,25 - DECÁMETRO CÚBICO,26 - METRO CÚBICO,27 - DECÍMETRO CÚBICO,28 - CENTÍMETRO CÚBICO,29 - MILÍMETRO CÚBICO,30 - HECTÓMETRO,31 - DECÁMETRO,32 - DECÍMETRO,33 - MILÍMETRO,34 - HECTOGRAMO,35 - DECAGRAMO,36 - DECIGRAMO,37 - CENTIGRAMO,38 - MILIGRAMO,39 - KILOLITRO,40 - HECTOLITRO,41 - DECALITRO,42 - DECILITRO,"</formula1>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="list">
+      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD,14 - CENTILITRO,15 - MILILITRO,16 - KILÓMETRO CUADRADO,17 - HECTÓMETRO CUADRADO,18 - DECÁMETRO CUADRADO,19 - METRO CUADRADO,20 - DECÍMETRO CUADRADO,21 - CENTÍMETRO CUADRADO,22 - MILÍMETRO CUADRADO,23 - KILÓMETRO CÚBICO,24 - HECTÓMETRO CÚBICO,25 - DECÁMETRO CÚBICO,26 - METRO CÚBICO,27 - DECÍMETRO CÚBICO,28 - CENTÍMETRO CÚBICO,29 - MILÍMETRO CÚBICO,30 - HECTÓMETRO,31 - DECÁMETRO,32 - DECÍMETRO,33 - MILÍMETRO,34 - HECTOGRAMO,35 - DECAGRAMO,36 - DECIGRAMO,37 - CENTIGRAMO,38 - MILIGRAMO,39 - KILOLITRO,40 - HECTOLITRO,41 - DECALITRO,42 - DECILITRO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -456,17 +452,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>